<commit_message>
Add subscription, organization, webhook routes to Vercel API
</commit_message>
<xml_diff>
--- a/めも/メモ.xlsx
+++ b/めも/メモ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shigemorishinji/Programming/claudecode/task/めも/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9FD8A42-3537-F44C-922B-8DF661C6BCA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{248400DC-1976-5342-A0A6-3B858940E80A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="1840" windowWidth="28300" windowHeight="17360" xr2:uid="{1EA390B4-7144-834D-867B-8977E05C585D}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="25600" windowHeight="15960" xr2:uid="{1EA390B4-7144-834D-867B-8977E05C585D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,9 +35,66 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>Supabaseアカウント作成</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>Shishi0918's Org</t>
+  </si>
+  <si>
+    <t>Project name</t>
+  </si>
+  <si>
+    <t>Database password</t>
+  </si>
+  <si>
+    <t>Shishi0918's Project</t>
+  </si>
+  <si>
+    <t>hfgTYG564fgfd$$gfd</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://supabase.com/dashboard/project/mwewfabykeyjopbeqbfj</t>
+  </si>
+  <si>
+    <t>URL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://vercel.com/</t>
+  </si>
+  <si>
+    <t>vercel</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>stripe</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>hfgdyRTvxc527$f</t>
+  </si>
+  <si>
+    <t>shinji19750918@yahoo.co.jp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -48,6 +105,35 @@
     </font>
     <font>
       <sz val="6"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF800000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF171717"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Yu Gothic"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
@@ -71,17 +157,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -414,13 +516,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5EEEF9-CA56-0847-8888-15489916DAEC}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="59" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1"/>
+  <hyperlinks>
+    <hyperlink ref="C11" r:id="rId1" xr:uid="{13625A9D-B339-C549-8B22-14D36E76913E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add hierarchical task structure with drag-and-drop nesting
- Add parent-child relationships to tasks (up to 3 levels)
- Implement drag-to-nest (drop on task name) and drag-to-unnest (drop on left edge)
- Add visual feedback: green for nest target, yellow for unnest mode
- Update SpotTask with parentId in database schema
- Add hierarchy support to SpotTaskCreatorPage with auto-save
- Add hierarchy support to MonthlyTemplateCreatorPage (localStorage)
- Add hierarchy support to YearlyTaskCreatorPage (localStorage)
- Update CalendarPage to display hierarchical tasks

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/めも/メモ.xlsx
+++ b/めも/メモ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shigemorishinji/Programming/claudecode/task/めも/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Programming\claudecode\task\めも\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{248400DC-1976-5342-A0A6-3B858940E80A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38452B48-4D91-4F9C-BFCD-98F71A809874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="25600" windowHeight="15960" xr2:uid="{1EA390B4-7144-834D-867B-8977E05C585D}"/>
+    <workbookView xWindow="-120" yWindow="255" windowWidth="29040" windowHeight="16065" xr2:uid="{1EA390B4-7144-834D-867B-8977E05C585D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Supabaseアカウント作成</t>
   </si>
@@ -87,6 +87,14 @@
   </si>
   <si>
     <t>shinji19750918@yahoo.co.jp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>shinji19750918@yahoo.co.jp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>password123</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -94,7 +102,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -139,6 +147,12 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10.8"/>
+      <color rgb="FFA31515"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -165,7 +179,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -180,6 +194,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -516,15 +536,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5EEEF9-CA56-0847-8888-15489916DAEC}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="19.899999999999999"/>
   <cols>
     <col min="2" max="2" width="59" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -532,7 +553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" ht="20.25">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -540,7 +561,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" ht="20.25">
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -548,7 +569,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" ht="20.25">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -556,7 +577,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" ht="20.25">
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
@@ -594,10 +615,27 @@
         <v>14</v>
       </c>
     </row>
+    <row r="14" spans="1:3" ht="59.65">
+      <c r="B14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="28.5">
+      <c r="B15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <hyperlinks>
     <hyperlink ref="C11" r:id="rId1" xr:uid="{13625A9D-B339-C549-8B22-14D36E76913E}"/>
+    <hyperlink ref="C14" r:id="rId2" xr:uid="{6F6A8DD2-A3B6-48C1-A14A-49C5B5B025B1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Auto backup: 2025-12-20 22:00
</commit_message>
<xml_diff>
--- a/めも/メモ.xlsx
+++ b/めも/メモ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Programming\claudecode\task\めも\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38452B48-4D91-4F9C-BFCD-98F71A809874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B596F10-8E7C-434A-9AD5-8AF87946EA7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="255" windowWidth="29040" windowHeight="16065" xr2:uid="{1EA390B4-7144-834D-867B-8977E05C585D}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
-  <si>
-    <t>Supabaseアカウント作成</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Organization</t>
   </si>
@@ -60,41 +57,67 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>URL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://vercel.com/</t>
+  </si>
+  <si>
+    <t>vercel</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>stripe</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>hfgdyRTvxc527$f</t>
+  </si>
+  <si>
+    <t>shinji19750918@yahoo.co.jp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>shinji19750918@yahoo.co.jp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>password123</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>https://supabase.com/dashboard/project/mwewfabykeyjopbeqbfj</t>
-  </si>
-  <si>
-    <t>URL</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>https://vercel.com/</t>
-  </si>
-  <si>
-    <t>vercel</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>stripe</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>hfgdyRTvxc527$f</t>
-  </si>
-  <si>
-    <t>shinji19750918@yahoo.co.jp</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>shinji19750918@yahoo.co.jp</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>password123</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>Supabase</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF800000"/>
+        <rFont val="ＭＳ ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>アカウント作成</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ログイン</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GITHUBでログイン　GITのＩＤ、PASSはアプリから</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -102,7 +125,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -152,6 +175,14 @@
       <color rgb="FFA31515"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF800000"/>
+      <name val="ＭＳ ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="2">
@@ -536,106 +567,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5EEEF9-CA56-0847-8888-15489916DAEC}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="19.899999999999999"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="19.5"/>
   <cols>
     <col min="2" max="2" width="59" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="20.25">
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="20.25">
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1"/>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="20.25">
       <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="20.25">
       <c r="B5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="20.25">
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="20.25">
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="11" spans="1:3">
+      <c r="C11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+    <row r="13" spans="1:3">
+      <c r="A13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="3" t="s">
+      <c r="C13" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="4" t="s">
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="59.65">
-      <c r="B14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="28.5">
-      <c r="B15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" xr:uid="{13625A9D-B339-C549-8B22-14D36E76913E}"/>
-    <hyperlink ref="C14" r:id="rId2" xr:uid="{6F6A8DD2-A3B6-48C1-A14A-49C5B5B025B1}"/>
+    <hyperlink ref="C13" r:id="rId1" xr:uid="{13625A9D-B339-C549-8B22-14D36E76913E}"/>
+    <hyperlink ref="C16" r:id="rId2" xr:uid="{6F6A8DD2-A3B6-48C1-A14A-49C5B5B025B1}"/>
+    <hyperlink ref="C7" r:id="rId3" xr:uid="{A09D61CD-9D31-4C0C-936E-DCA1B94D3D72}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix: Use Prisma singleton pattern for serverless
Created prisma.ts utility with singleton pattern to prevent
connection pool exhaustion in Vercel serverless environment.

Updated all controllers to use the shared prisma instance.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/めも/メモ.xlsx
+++ b/めも/メモ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Programming\claudecode\task\めも\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B596F10-8E7C-434A-9AD5-8AF87946EA7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB94ECC-EDD0-48D0-918D-ADE447CCC953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="255" windowWidth="29040" windowHeight="16065" xr2:uid="{1EA390B4-7144-834D-867B-8977E05C585D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Organization</t>
   </si>
@@ -51,10 +51,6 @@
   </si>
   <si>
     <t>Shishi0918's Project</t>
-  </si>
-  <si>
-    <t>hfgTYG564fgfd$$gfd</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>URL</t>
@@ -120,12 +116,39 @@
     <t>GITHUBでログイン　GITのＩＤ、PASSはアプリから</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>hgtunb26364AQK</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF171717"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>注意点</t>
+    </r>
+    <rPh sb="0" eb="3">
+      <t>チュウイテン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>バーセルからのdb接続urlはtransaction poolerにする。DirctはNG</t>
+    <rPh sb="9" eb="11">
+      <t>セツゾク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -182,6 +205,13 @@
       <color rgb="FF800000"/>
       <name val="ＭＳ ゴシック"/>
       <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF171717"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
       <charset val="128"/>
     </font>
   </fonts>
@@ -570,7 +600,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="19.5"/>
@@ -581,16 +611,16 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
         <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -617,61 +647,69 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="20.25">
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="25.5">
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="C11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="C13" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="B16" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="2:3">
       <c r="B17" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto backup: 2025-12-21 03:00
</commit_message>
<xml_diff>
--- a/めも/メモ.xlsx
+++ b/めも/メモ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Programming\claudecode\task\めも\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB94ECC-EDD0-48D0-918D-ADE447CCC953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF22561-DC4D-4294-BE2E-E8323E11EBAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="255" windowWidth="29040" windowHeight="16065" xr2:uid="{1EA390B4-7144-834D-867B-8977E05C585D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>Organization</t>
   </si>
@@ -141,6 +141,107 @@
     <rPh sb="9" eb="11">
       <t>セツゾク</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>環境変数の設定</t>
+    <rPh sb="0" eb="2">
+      <t>カンキョウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ヘンスウ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>settingから行うが、チーム画面に勝手になるので超注意。
+Settingボタンを押し、左上の上と下の記号をおして、task-managerを選択するとProjectSettingの表示になる。Settingだとだめ</t>
+    <rPh sb="9" eb="10">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>カッテ</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>チョウ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>チュウイ</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t>ヒダリ</t>
+    </rPh>
+    <rPh sb="46" eb="47">
+      <t>ウエ</t>
+    </rPh>
+    <rPh sb="48" eb="49">
+      <t>ウエ</t>
+    </rPh>
+    <rPh sb="50" eb="51">
+      <t>シタ</t>
+    </rPh>
+    <rPh sb="52" eb="54">
+      <t>キゴウ</t>
+    </rPh>
+    <rPh sb="72" eb="74">
+      <t>センタク</t>
+    </rPh>
+    <rPh sb="92" eb="94">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テストID</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Pass</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dgfhyt6543g</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>めーる</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bbbb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>zxjfurhjvc@yahoo.co.jp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>vndhry@yahoo.co.jp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CCCC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dhfjt6534</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>shishi0918</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -240,7 +341,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -261,6 +362,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -597,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5EEEF9-CA56-0847-8888-15489916DAEC}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="19.5"/>
@@ -676,48 +780,134 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:3" ht="58.5">
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3" t="s">
+    <row r="16" spans="1:3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="B16" s="3" t="s">
+    <row r="18" spans="1:3">
+      <c r="B18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
-      <c r="B17" s="3" t="s">
+    <row r="19" spans="1:3">
+      <c r="B19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C19" s="5" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="B22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="B23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="B25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="B26" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="B27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="B29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="B30" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="B31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <hyperlinks>
-    <hyperlink ref="C13" r:id="rId1" xr:uid="{13625A9D-B339-C549-8B22-14D36E76913E}"/>
-    <hyperlink ref="C16" r:id="rId2" xr:uid="{6F6A8DD2-A3B6-48C1-A14A-49C5B5B025B1}"/>
+    <hyperlink ref="C15" r:id="rId1" xr:uid="{13625A9D-B339-C549-8B22-14D36E76913E}"/>
+    <hyperlink ref="C18" r:id="rId2" xr:uid="{6F6A8DD2-A3B6-48C1-A14A-49C5B5B025B1}"/>
     <hyperlink ref="C7" r:id="rId3" xr:uid="{A09D61CD-9D31-4C0C-936E-DCA1B94D3D72}"/>
+    <hyperlink ref="C21" r:id="rId4" xr:uid="{1EBCA35B-47A4-4CD5-B7CA-18826254181E}"/>
+    <hyperlink ref="C25" r:id="rId5" xr:uid="{FE797399-172A-466A-8AE2-FA6C718FA082}"/>
+    <hyperlink ref="C29" r:id="rId6" xr:uid="{A37F03F2-D37F-4261-B825-D4DED068E99A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Auto backup: 2025-12-21 16:00
</commit_message>
<xml_diff>
--- a/めも/メモ.xlsx
+++ b/めも/メモ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Programming\claudecode\task\めも\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF22561-DC4D-4294-BE2E-E8323E11EBAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978B559C-C03C-410A-A91C-0BE9C2C6D4B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="255" windowWidth="29040" windowHeight="16065" xr2:uid="{1EA390B4-7144-834D-867B-8977E05C585D}"/>
+    <workbookView xWindow="-195" yWindow="180" windowWidth="29190" windowHeight="16215" xr2:uid="{1EA390B4-7144-834D-867B-8977E05C585D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>Organization</t>
   </si>
@@ -242,6 +242,18 @@
   </si>
   <si>
     <t>shishi0918</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>gkrunrufjut@yahoo.co.jp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DDD</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>hfjethsfdhjfkht</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -701,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5EEEF9-CA56-0847-8888-15489916DAEC}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="19.5"/>
@@ -899,6 +911,30 @@
         <v>34</v>
       </c>
     </row>
+    <row r="33" spans="2:3">
+      <c r="B33" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="B34" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <hyperlinks>
@@ -908,6 +944,7 @@
     <hyperlink ref="C21" r:id="rId4" xr:uid="{1EBCA35B-47A4-4CD5-B7CA-18826254181E}"/>
     <hyperlink ref="C25" r:id="rId5" xr:uid="{FE797399-172A-466A-8AE2-FA6C718FA082}"/>
     <hyperlink ref="C29" r:id="rId6" xr:uid="{A37F03F2-D37F-4261-B825-D4DED068E99A}"/>
+    <hyperlink ref="C33" r:id="rId7" xr:uid="{0A484C4E-8488-4705-AD43-B861AF7B4887}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>